<commit_message>
Update RELAÇÃO DE FISCAIS DE CONTRATOS VIGENTES.xlsx
</commit_message>
<xml_diff>
--- a/RELAÇÃO DE FISCAIS DE CONTRATOS VIGENTES.xlsx
+++ b/RELAÇÃO DE FISCAIS DE CONTRATOS VIGENTES.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Compras\Desktop\2025\GEOBRAS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Compras\Documents\GitHub\patrimonio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D064F89B-9858-49E5-83ED-C2FB9C2A979C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{837D3673-5759-4613-AFC1-05208757135D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$B$3:$H$64</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Plan1!$1:$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="155">
   <si>
     <t>RELAÇÃO DE FISCAIS DE CONTRATOS VIGENTES</t>
   </si>
@@ -461,6 +461,36 @@
   </si>
   <si>
     <t>NÃO</t>
+  </si>
+  <si>
+    <t>nro</t>
+  </si>
+  <si>
+    <t>empresa</t>
+  </si>
+  <si>
+    <t>tipo</t>
+  </si>
+  <si>
+    <t>FC</t>
+  </si>
+  <si>
+    <t>FCS</t>
+  </si>
+  <si>
+    <t>FO</t>
+  </si>
+  <si>
+    <t>FOS</t>
+  </si>
+  <si>
+    <t>VALOR CONTRATO</t>
+  </si>
+  <si>
+    <t>VALOR PAGO</t>
+  </si>
+  <si>
+    <t>SALDO</t>
   </si>
 </sst>
 </file>
@@ -541,7 +571,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -558,16 +588,18 @@
     <xf numFmtId="17" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -877,9 +909,9 @@
   </sheetPr>
   <dimension ref="A1:H216"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A58" sqref="A58"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,29 +940,29 @@
       <c r="A2" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6" t="s">
+      <c r="F2" s="9"/>
+      <c r="G2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="6"/>
+      <c r="H2" s="9"/>
     </row>
     <row r="3" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
       <c r="E3" s="3" t="s">
         <v>130</v>
       </c>
@@ -945,7 +977,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -971,7 +1003,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -997,7 +1029,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1023,7 +1055,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1049,7 +1081,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1075,7 +1107,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1101,7 +1133,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1127,7 +1159,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -1153,7 +1185,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1179,7 +1211,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1205,7 +1237,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1231,7 +1263,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -1257,7 +1289,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1283,7 +1315,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -1309,7 +1341,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1335,7 +1367,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -1361,7 +1393,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1387,7 +1419,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -1413,7 +1445,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -1439,7 +1471,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1465,7 +1497,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -1491,7 +1523,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1517,7 +1549,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B26" s="4" t="s">
@@ -1543,7 +1575,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -1569,7 +1601,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -1595,7 +1627,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -1621,7 +1653,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B30" s="4" t="s">
@@ -1647,7 +1679,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -1673,7 +1705,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B32" s="4" t="s">
@@ -1699,7 +1731,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -1725,7 +1757,7 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -1751,7 +1783,7 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B35" s="4" t="s">
@@ -1777,7 +1809,7 @@
       </c>
     </row>
     <row r="36" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -1803,7 +1835,7 @@
       </c>
     </row>
     <row r="37" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="s">
+      <c r="A37" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -1829,7 +1861,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
+      <c r="A38" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -1855,7 +1887,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
+      <c r="A39" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B39" s="2" t="s">
@@ -1881,7 +1913,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -1907,7 +1939,7 @@
       </c>
     </row>
     <row r="41" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
+      <c r="A41" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -1933,7 +1965,7 @@
       </c>
     </row>
     <row r="42" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="9" t="s">
+      <c r="A42" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -1959,7 +1991,7 @@
       </c>
     </row>
     <row r="43" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="9" t="s">
+      <c r="A43" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B43" s="2" t="s">
@@ -1985,7 +2017,7 @@
       </c>
     </row>
     <row r="44" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="9" t="s">
+      <c r="A44" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -2011,7 +2043,7 @@
       </c>
     </row>
     <row r="45" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="9" t="s">
+      <c r="A45" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -2037,7 +2069,7 @@
       </c>
     </row>
     <row r="46" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="9" t="s">
+      <c r="A46" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B46" s="2" t="s">
@@ -2063,7 +2095,7 @@
       </c>
     </row>
     <row r="47" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="9" t="s">
+      <c r="A47" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B47" s="2" t="s">
@@ -2089,7 +2121,7 @@
       </c>
     </row>
     <row r="48" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="9" t="s">
+      <c r="A48" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B48" s="2" t="s">
@@ -2115,7 +2147,7 @@
       </c>
     </row>
     <row r="49" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="9" t="s">
+      <c r="A49" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B49" s="2" t="s">
@@ -2141,7 +2173,7 @@
       </c>
     </row>
     <row r="50" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="9" t="s">
+      <c r="A50" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -2167,7 +2199,7 @@
       </c>
     </row>
     <row r="51" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="9" t="s">
+      <c r="A51" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B51" s="2" t="s">
@@ -2193,7 +2225,7 @@
       </c>
     </row>
     <row r="52" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="9" t="s">
+      <c r="A52" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B52" s="2" t="s">
@@ -2219,7 +2251,7 @@
       </c>
     </row>
     <row r="53" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="9" t="s">
+      <c r="A53" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B53" s="2" t="s">
@@ -2245,7 +2277,7 @@
       </c>
     </row>
     <row r="54" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="9" t="s">
+      <c r="A54" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B54" s="2" t="s">
@@ -2271,7 +2303,7 @@
       </c>
     </row>
     <row r="55" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="9" t="s">
+      <c r="A55" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B55" s="2" t="s">
@@ -2297,7 +2329,7 @@
       </c>
     </row>
     <row r="56" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="9" t="s">
+      <c r="A56" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B56" s="2" t="s">
@@ -2323,7 +2355,7 @@
       </c>
     </row>
     <row r="57" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="9" t="s">
+      <c r="A57" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B57" s="2" t="s">
@@ -2349,7 +2381,7 @@
       </c>
     </row>
     <row r="58" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="9" t="s">
+      <c r="A58" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B58" s="2" t="s">
@@ -2375,7 +2407,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="9" t="s">
+      <c r="A59" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B59" s="2" t="s">
@@ -2401,7 +2433,7 @@
       </c>
     </row>
     <row r="60" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="9" t="s">
+      <c r="A60" s="6" t="s">
         <v>143</v>
       </c>
       <c r="B60" s="2" t="s">
@@ -2427,7 +2459,7 @@
       </c>
     </row>
     <row r="61" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="9" t="s">
+      <c r="A61" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B61" s="2" t="s">
@@ -2453,7 +2485,7 @@
       </c>
     </row>
     <row r="62" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="9" t="s">
+      <c r="A62" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B62" s="2" t="s">
@@ -2479,7 +2511,7 @@
       </c>
     </row>
     <row r="63" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="9" t="s">
+      <c r="A63" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B63" s="2" t="s">
@@ -2505,7 +2537,7 @@
       </c>
     </row>
     <row r="64" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="9" t="s">
+      <c r="A64" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B64" s="2" t="s">
@@ -3010,12 +3042,1596 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A3:J65"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="17.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E3" t="s">
+        <v>149</v>
+      </c>
+      <c r="F3" t="s">
+        <v>150</v>
+      </c>
+      <c r="G3" t="s">
+        <v>151</v>
+      </c>
+      <c r="H3" t="s">
+        <v>152</v>
+      </c>
+      <c r="I3" t="s">
+        <v>153</v>
+      </c>
+      <c r="J3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H6" s="11">
+        <v>274770</v>
+      </c>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H10" s="11">
+        <v>5076431.47</v>
+      </c>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="H12" s="11">
+        <v>5310660</v>
+      </c>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="H16" s="11">
+        <v>2328943.1</v>
+      </c>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="H20" s="11">
+        <v>415994.99</v>
+      </c>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="H21" s="11">
+        <v>1311577.5</v>
+      </c>
+      <c r="I21" s="11">
+        <v>1224279.8700000001</v>
+      </c>
+      <c r="J21" s="11"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H22" s="11">
+        <v>988060.58</v>
+      </c>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H23" s="11">
+        <v>621000</v>
+      </c>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="H24" s="11">
+        <v>1496880</v>
+      </c>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="H25" s="11">
+        <v>1943588.94</v>
+      </c>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H26" s="11">
+        <v>192000</v>
+      </c>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="H32" s="11">
+        <v>1902400</v>
+      </c>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H33" s="11">
+        <v>4236574.88</v>
+      </c>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="H35" s="11">
+        <v>3297283.23</v>
+      </c>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="H38" s="11">
+        <v>4149472.94</v>
+      </c>
+      <c r="I38" s="11">
+        <v>1898820.3</v>
+      </c>
+      <c r="J38" s="11"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H40" s="11"/>
+      <c r="I40" s="11">
+        <v>135000</v>
+      </c>
+      <c r="J40" s="11"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="H41" s="11">
+        <v>10004185.199999999</v>
+      </c>
+      <c r="I41" s="11"/>
+      <c r="J41" s="11"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H42" s="11">
+        <v>737000</v>
+      </c>
+      <c r="I42" s="11"/>
+      <c r="J42" s="11"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H43" s="11"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="11"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="H44" s="11">
+        <v>590000</v>
+      </c>
+      <c r="I44" s="11"/>
+      <c r="J44" s="11"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="11"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H46" s="11"/>
+      <c r="I46" s="11"/>
+      <c r="J46" s="11"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H47" s="11"/>
+      <c r="I47" s="11"/>
+      <c r="J47" s="11"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="H48" s="11"/>
+      <c r="I48" s="11"/>
+      <c r="J48" s="11"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="H49" s="11">
+        <v>1357500</v>
+      </c>
+      <c r="I49" s="11"/>
+      <c r="J49" s="11"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="11"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H51" s="11">
+        <v>3270384.36</v>
+      </c>
+      <c r="I51" s="11"/>
+      <c r="J51" s="11"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H52" s="11"/>
+      <c r="I52" s="11"/>
+      <c r="J52" s="11"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H53" s="11"/>
+      <c r="I53" s="11"/>
+      <c r="J53" s="11"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="H54" s="11"/>
+      <c r="I54" s="11"/>
+      <c r="J54" s="11"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="H55" s="11"/>
+      <c r="I55" s="11"/>
+      <c r="J55" s="11"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="H56" s="11"/>
+      <c r="I56" s="11"/>
+      <c r="J56" s="11"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H57" s="11"/>
+      <c r="I57" s="11"/>
+      <c r="J57" s="11"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H58" s="11">
+        <v>705600</v>
+      </c>
+      <c r="I58" s="11"/>
+      <c r="J58" s="11"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H59" s="11">
+        <v>108303.03999999999</v>
+      </c>
+      <c r="I59" s="11"/>
+      <c r="J59" s="11"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H60" s="11"/>
+      <c r="I60" s="11"/>
+      <c r="J60" s="11"/>
+    </row>
+    <row r="65" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H65" s="10">
+        <f>SUM(H59,H58,H42,H41,H33,H32,H26,H23,H22,H21,H20,H16,H12,H10,H6)</f>
+        <v>34213500.759999998</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>

</xml_diff>